<commit_message>
Addiction DictionaryBase class and Spanish Terms test
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-dictionary.xlsx
+++ b/test-data/webanalytics-dictionary.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{6CD2B263-7F12-4B56-8242-74A0B392AA88}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{173D06B2-359C-4474-AB11-70B6A502BC5A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DictionaryPage" sheetId="11" r:id="rId1"/>
     <sheet name="DictionaryPopup" sheetId="12" r:id="rId2"/>
+    <sheet name="TermsSpanish" sheetId="13" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="24">
   <si>
     <t>Path</t>
   </si>
@@ -83,6 +84,21 @@
   </si>
   <si>
     <t>Dictionary Popup</t>
+  </si>
+  <si>
+    <t>Dictionary Page</t>
+  </si>
+  <si>
+    <t>Dictionary Search Page</t>
+  </si>
+  <si>
+    <t>Dictionary Page Expand</t>
+  </si>
+  <si>
+    <t>/espanol/publicaciones/diccionario/buscar</t>
+  </si>
+  <si>
+    <t>/espanol/publicaciones/diccionario?expand=D</t>
   </si>
 </sst>
 </file>
@@ -451,7 +467,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E2B4AE-FC4B-430F-8D43-76B5FBC9E609}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -544,7 +560,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection sqref="A1:B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,4 +612,55 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A26FFB-8745-44DF-9216-1D60F2C8BF67}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Added Drug, English Term test classes
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-dictionary.xlsx
+++ b/test-data/webanalytics-dictionary.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{90507CB9-9C73-4308-A66E-1F42CE5DB01E}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C701F614-1C96-478E-ABE9-6F13DDDAA1C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="14" r:id="rId1"/>
     <sheet name="DictionaryPage" sheetId="11" r:id="rId2"/>
     <sheet name="DictionaryPopup" sheetId="12" r:id="rId3"/>
-    <sheet name="TermsSpanish" sheetId="13" r:id="rId4"/>
+    <sheet name="TermsEnglish" sheetId="15" r:id="rId4"/>
+    <sheet name="TermsSpanish" sheetId="13" r:id="rId5"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
   <si>
     <t>Path</t>
   </si>
@@ -54,18 +55,12 @@
     <t>/publications/dictionaries/cancer-terms/search?contains=true&amp;q=breast</t>
   </si>
   <si>
-    <t>Term Dictionary</t>
-  </si>
-  <si>
     <t>Drug Dictionary</t>
   </si>
   <si>
     <t>Genetics Dictionary</t>
   </si>
   <si>
-    <t>Dictionary Search</t>
-  </si>
-  <si>
     <t>/common/popUps/popDefinition.aspx?id=CDR0000045788&amp;version=patient&amp;language=English&amp;dictionary=Cancer.gov</t>
   </si>
   <si>
@@ -157,6 +152,15 @@
   </si>
   <si>
     <t>Drug|English|F 18 fluorodeoxygalactose|687016</t>
+  </si>
+  <si>
+    <t>/espanol/publicaciones/diccionario/buscar?contains=true&amp;q=tumor</t>
+  </si>
+  <si>
+    <t>Dictionary Contains</t>
+  </si>
+  <si>
+    <t>/publications/dictionaries/cancer-terms/search</t>
   </si>
 </sst>
 </file>
@@ -525,7 +529,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE78283C-AF97-40C5-A687-7F3B70984468}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -541,98 +545,98 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C2" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>31</v>
+      </c>
+      <c r="B8" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" t="s">
         <v>33</v>
-      </c>
-      <c r="B8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C8" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" t="s">
         <v>34</v>
-      </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -643,15 +647,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E2B4AE-FC4B-430F-8D43-76B5FBC9E609}">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:B3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A22" sqref="A22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="67.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.140625" customWidth="1"/>
     <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -665,7 +669,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
         <v>8</v>
@@ -673,42 +677,10 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
         <v>9</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -741,34 +713,34 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -777,8 +749,8 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A26FFB-8745-44DF-9216-1D60F2C8BF67}">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FD43C8-074C-454D-B3D5-D4C587E6FC69}">
+  <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
@@ -786,7 +758,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="43.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="67.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -800,26 +772,93 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>19</v>
+        <v>43</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A26FFB-8745-44DF-9216-1D60F2C8BF67}">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="63" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
         <v>18</v>
+      </c>
+      <c r="B4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>41</v>
+      </c>
+      <c r="B5" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added Genetics Dictionary tests
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-dictionary.xlsx
+++ b/test-data/webanalytics-dictionary.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{C701F614-1C96-478E-ABE9-6F13DDDAA1C1}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{56553169-964E-4504-A396-EB317B35D4B7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="14" r:id="rId1"/>
-    <sheet name="DictionaryPage" sheetId="11" r:id="rId2"/>
-    <sheet name="DictionaryPopup" sheetId="12" r:id="rId3"/>
+    <sheet name="DictionaryPopup" sheetId="12" r:id="rId2"/>
+    <sheet name="TermsDrugs" sheetId="16" r:id="rId3"/>
     <sheet name="TermsEnglish" sheetId="15" r:id="rId4"/>
-    <sheet name="TermsSpanish" sheetId="13" r:id="rId5"/>
+    <sheet name="TermsGenetics" sheetId="11" r:id="rId5"/>
+    <sheet name="TermsSpanish" sheetId="13" r:id="rId6"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
   <si>
     <t>Path</t>
   </si>
@@ -55,12 +56,6 @@
     <t>/publications/dictionaries/cancer-terms/search?contains=true&amp;q=breast</t>
   </si>
   <si>
-    <t>Drug Dictionary</t>
-  </si>
-  <si>
-    <t>Genetics Dictionary</t>
-  </si>
-  <si>
     <t>/common/popUps/popDefinition.aspx?id=CDR0000045788&amp;version=patient&amp;language=English&amp;dictionary=Cancer.gov</t>
   </si>
   <si>
@@ -161,6 +156,18 @@
   </si>
   <si>
     <t>/publications/dictionaries/cancer-terms/search</t>
+  </si>
+  <si>
+    <t>/publications/dictionaries/cancer-drug/search?contains=false&amp;q=interferon</t>
+  </si>
+  <si>
+    <t>/publications/dictionaries/cancer-drug?expand=J</t>
+  </si>
+  <si>
+    <t>/publications/dictionaries/genetics-dictionary?expand=K</t>
+  </si>
+  <si>
+    <t>/publications/dictionaries/genetics-dictionary/search?contains=false&amp;q=genom</t>
   </si>
 </sst>
 </file>
@@ -545,98 +552,98 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C6" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C7" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" t="s">
         <v>31</v>
-      </c>
-      <c r="B8" t="s">
-        <v>22</v>
-      </c>
-      <c r="C8" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
+        <v>30</v>
+      </c>
+      <c r="B9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" t="s">
         <v>32</v>
-      </c>
-      <c r="B9" t="s">
-        <v>22</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
       </c>
     </row>
   </sheetData>
@@ -646,55 +653,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E2B4AE-FC4B-430F-8D43-76B5FBC9E609}">
-  <dimension ref="A1:B3"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="43.140625" customWidth="1"/>
-    <col min="2" max="2" width="18.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B72C3B8-6F8A-4983-9AE2-1BC71D4D3FC5}">
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B2"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -713,38 +676,90 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" t="s">
         <v>11</v>
-      </c>
-      <c r="B3" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75059FB7-20C9-43F2-BD8A-12F5958F43A9}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
       </c>
       <c r="B4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -753,7 +768,7 @@
   <dimension ref="A1:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -775,15 +790,15 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -791,7 +806,7 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -799,7 +814,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -808,6 +823,58 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E2B4AE-FC4B-430F-8D43-76B5FBC9E609}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="74" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A26FFB-8745-44DF-9216-1D60F2C8BF67}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -834,31 +901,31 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start building dictionary search click tests
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-dictionary.xlsx
+++ b/test-data/webanalytics-dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{56553169-964E-4504-A396-EB317B35D4B7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B7418C97-C4E2-499F-BDF4-1B6A5223FDE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="14" r:id="rId1"/>
@@ -826,7 +826,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E2B4AE-FC4B-430F-8D43-76B5FBC9E609}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -878,7 +878,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A26FFB-8745-44DF-9216-1D60F2C8BF67}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Cleanup click test, added more data
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-dictionary.xlsx
+++ b/test-data/webanalytics-dictionary.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B7418C97-C4E2-499F-BDF4-1B6A5223FDE7}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5785E7CC-1327-438E-B168-8058D1DCAA49}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="14" r:id="rId1"/>
-    <sheet name="DictionaryPopup" sheetId="12" r:id="rId2"/>
-    <sheet name="TermsDrugs" sheetId="16" r:id="rId3"/>
-    <sheet name="TermsEnglish" sheetId="15" r:id="rId4"/>
-    <sheet name="TermsGenetics" sheetId="11" r:id="rId5"/>
-    <sheet name="TermsSpanish" sheetId="13" r:id="rId6"/>
+    <sheet name="SearchTerms" sheetId="17" r:id="rId2"/>
+    <sheet name="DictionaryPopup" sheetId="12" r:id="rId3"/>
+    <sheet name="TermsPageDrugs" sheetId="16" r:id="rId4"/>
+    <sheet name="TermsPageEnglish" sheetId="15" r:id="rId5"/>
+    <sheet name="TermsPageGenetics" sheetId="11" r:id="rId6"/>
+    <sheet name="TermsPageSpanish" sheetId="13" r:id="rId7"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -30,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
   <si>
     <t>Path</t>
   </si>
@@ -168,6 +169,15 @@
   </si>
   <si>
     <t>/publications/dictionaries/genetics-dictionary/search?contains=false&amp;q=genom</t>
+  </si>
+  <si>
+    <t>SearchTerm</t>
+  </si>
+  <si>
+    <t>LinkName</t>
+  </si>
+  <si>
+    <t>SearchType</t>
   </si>
 </sst>
 </file>
@@ -653,6 +663,64 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F3036A-4AA5-4DF4-B5A3-DBA7482C8C58}">
+  <dimension ref="A1:D4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="70.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B72C3B8-6F8A-4983-9AE2-1BC71D4D3FC5}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -711,12 +779,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75059FB7-20C9-43F2-BD8A-12F5958F43A9}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection sqref="A1:B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -763,7 +831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B5FD43C8-074C-454D-B3D5-D4C587E6FC69}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -822,7 +890,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{76E2B4AE-FC4B-430F-8D43-76B5FBC9E609}">
   <dimension ref="A1:B4"/>
   <sheetViews>
@@ -874,11 +942,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{71A26FFB-8745-44DF-9216-1D60F2C8BF67}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Added results click tests
</commit_message>
<xml_diff>
--- a/test-data/webanalytics-dictionary.xlsx
+++ b/test-data/webanalytics-dictionary.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Development\WCMS\qa-testing\test-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{5785E7CC-1327-438E-B168-8058D1DCAA49}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{04C8EEFB-A639-4B8F-A88A-9565010677D6}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12750" windowHeight="2640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Definitions" sheetId="14" r:id="rId1"/>
-    <sheet name="SearchTerms" sheetId="17" r:id="rId2"/>
-    <sheet name="DictionaryPopup" sheetId="12" r:id="rId3"/>
+    <sheet name="DictionaryPopup" sheetId="12" r:id="rId2"/>
+    <sheet name="SearchTerms" sheetId="17" r:id="rId3"/>
     <sheet name="TermsPageDrugs" sheetId="16" r:id="rId4"/>
     <sheet name="TermsPageEnglish" sheetId="15" r:id="rId5"/>
     <sheet name="TermsPageGenetics" sheetId="11" r:id="rId6"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="60">
   <si>
     <t>Path</t>
   </si>
@@ -178,6 +178,39 @@
   </si>
   <si>
     <t>SearchType</t>
+  </si>
+  <si>
+    <t>dictionary_terms</t>
+  </si>
+  <si>
+    <t>TermsDictionarySearch</t>
+  </si>
+  <si>
+    <t>breast</t>
+  </si>
+  <si>
+    <t>diccionario</t>
+  </si>
+  <si>
+    <t>tumor</t>
+  </si>
+  <si>
+    <t>DrugDictionarySearch</t>
+  </si>
+  <si>
+    <t>dictionary_drugs</t>
+  </si>
+  <si>
+    <t>herceptin</t>
+  </si>
+  <si>
+    <t>GeneticsDictionarySearch</t>
+  </si>
+  <si>
+    <t>dictionary_genetics</t>
+  </si>
+  <si>
+    <t>allele</t>
   </si>
 </sst>
 </file>
@@ -546,7 +579,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE78283C-AF97-40C5-A687-7F3B70984468}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -663,64 +696,6 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F3036A-4AA5-4DF4-B5A3-DBA7482C8C58}">
-  <dimension ref="A1:D4"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="70.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>42</v>
-      </c>
-      <c r="B4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B72C3B8-6F8A-4983-9AE2-1BC71D4D3FC5}">
   <dimension ref="A1:B5"/>
   <sheetViews>
@@ -779,12 +754,104 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81F3036A-4AA5-4DF4-B5A3-DBA7482C8C58}">
+  <dimension ref="A1:D5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="43" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>56</v>
+      </c>
+      <c r="C4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D4" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>59</v>
+      </c>
+      <c r="C5" t="s">
+        <v>58</v>
+      </c>
+      <c r="D5" t="s">
+        <v>57</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="90" verticalDpi="90" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{75059FB7-20C9-43F2-BD8A-12F5958F43A9}">
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B4"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>